<commit_message>
added labels and saved figures
</commit_message>
<xml_diff>
--- a/Data/EU_em.xlsx
+++ b/Data/EU_em.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacEvans\Documents\Uni\AI\EV_affect_on_emissions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDA43D7-91E5-4424-BE8C-7AF0CAFF136B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E4FB31-BE9A-4703-B4EB-C25F3326BE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Data" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M587"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26602,6 +26602,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001D2B3AC84071846ACF4D55F98677E20" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d240198b7d04cb6b94fdaf1066024223">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="13f50ba1-f9d4-4561-9ce6-901d3df2835b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c9dc931702eb9c0d27bdf68ea8bd3e9" ns2:_="">
     <xsd:import namespace="13f50ba1-f9d4-4561-9ce6-901d3df2835b"/>
@@ -26747,22 +26762,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3623FC5-ECEF-41DD-AB06-D15C0B1AF150}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0630A7F-21BA-403E-A17D-B117E7686FE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94E410D1-5E0A-4A84-8E96-AAF0E0A826AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26778,21 +26795,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0630A7F-21BA-403E-A17D-B117E7686FE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3623FC5-ECEF-41DD-AB06-D15C0B1AF150}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>